<commit_message>
added a new function: pilesupport
</commit_message>
<xml_diff>
--- a/testing/lumpedmass.xlsx
+++ b/testing/lumpedmass.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="lumpedmass" sheetId="1" r:id="rId1"/>
     <sheet name="framestructure" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="pilesupport" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="164">
   <si>
     <t>\baseslabw</t>
   </si>
@@ -451,24 +451,6 @@
     <t>\axisseperation</t>
   </si>
   <si>
-    <t xml:space="preserve">\showpiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\numberofpiles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\piledepth </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\pilesidespace </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\pilediameter </t>
-  </si>
-  <si>
-    <t xml:space="preserve">\pilelinethickness </t>
-  </si>
-  <si>
     <t>show piles</t>
   </si>
   <si>
@@ -503,6 +485,39 @@
   </si>
   <si>
     <t>\pilelinethickness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>\coordinatex</t>
+  </si>
+  <si>
+    <t>\coordinatey</t>
+  </si>
+  <si>
+    <t>\pdepth</t>
+  </si>
+  <si>
+    <t>\pdiameter</t>
+  </si>
+  <si>
+    <t>\plinethick</t>
+  </si>
+  <si>
+    <t>x coordinate</t>
+  </si>
+  <si>
+    <t>y coordinate</t>
+  </si>
+  <si>
+    <t>fill color</t>
+  </si>
+  <si>
+    <t>\fillcolor</t>
+  </si>
+  <si>
+    <t>gray</t>
   </si>
 </sst>
 </file>
@@ -872,11 +887,11 @@
         <v>29</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE(A2,"=",C2,",")</f>
+        <f t="shared" ref="D2:D19" si="0">CONCATENATE(A2,"=",C2,",")</f>
         <v>base slab width=0.8cm,</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE(A2,"/.store in=", B2,",")</f>
+        <f t="shared" ref="E2:E19" si="1">CONCATENATE(A2,"/.store in=", B2,",")</f>
         <v>base slab width/.store in=\baseslabw,</v>
       </c>
       <c r="F2" t="str">
@@ -895,15 +910,15 @@
         <v>30</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE(A3,"=",C3,",")</f>
+        <f t="shared" si="0"/>
         <v>base slab height=0.3cm,</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE(A3,"/.store in=", B3,",")</f>
+        <f t="shared" si="1"/>
         <v>base slab height/.store in=\baseslabh,</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F19" si="0">CONCATENATE(B3,"=",B3,";")</f>
+        <f t="shared" ref="F3:F19" si="2">CONCATENATE(B3,"=",B3,";")</f>
         <v>\baseslabh=\baseslabh;</v>
       </c>
     </row>
@@ -918,15 +933,15 @@
         <v>31</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE(A4,"=",C4,",")</f>
+        <f t="shared" si="0"/>
         <v>foundation width=1cm,</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE(A4,"/.store in=", B4,",")</f>
+        <f t="shared" si="1"/>
         <v>foundation width/.store in=\foundationw,</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\foundationw=\foundationw;</v>
       </c>
     </row>
@@ -941,15 +956,15 @@
         <v>32</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE(A5,"=",C5,",")</f>
+        <f t="shared" si="0"/>
         <v>x axis length=0.5cm,</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE(A5,"/.store in=", B5,",")</f>
+        <f t="shared" si="1"/>
         <v>x axis length/.store in=\axeslenX,</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\axeslenX=\axeslenX;</v>
       </c>
     </row>
@@ -964,15 +979,15 @@
         <v>32</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE(A6,"=",C6,",")</f>
+        <f t="shared" si="0"/>
         <v>y axis length=0.5cm,</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE(A6,"/.store in=", B6,",")</f>
+        <f t="shared" si="1"/>
         <v>y axis length/.store in=\axeslenY,</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\axeslenY=\axeslenY;</v>
       </c>
     </row>
@@ -987,15 +1002,15 @@
         <v>33</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE(A7,"=",C7,",")</f>
+        <f t="shared" si="0"/>
         <v>drift distance=0.4cm,</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE(A7,"/.store in=", B7,",")</f>
+        <f t="shared" si="1"/>
         <v>drift distance/.store in=\driftdist,</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\driftdist=\driftdist;</v>
       </c>
     </row>
@@ -1010,15 +1025,15 @@
         <v>41</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE(A8,"=",C8,",")</f>
+        <f t="shared" si="0"/>
         <v>drift curve ratio=0.65,</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE(A8,"/.store in=", B8,",")</f>
+        <f t="shared" si="1"/>
         <v>drift curve ratio/.store in=\driftcurveratio,</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\driftcurveratio=\driftcurveratio;</v>
       </c>
     </row>
@@ -1033,15 +1048,15 @@
         <v>34</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE(A9,"=",C9,",")</f>
+        <f t="shared" si="0"/>
         <v>base slab drift=1.1cm,</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE(A9,"/.store in=", B9,",")</f>
+        <f t="shared" si="1"/>
         <v>base slab drift/.store in=\basedriftdist,</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\basedriftdist=\basedriftdist;</v>
       </c>
     </row>
@@ -1056,15 +1071,15 @@
         <v>35</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE(A10,"=",C10,",")</f>
+        <f t="shared" si="0"/>
         <v>foundation drift=2cm,</v>
       </c>
       <c r="E10" t="str">
-        <f>CONCATENATE(A10,"/.store in=", B10,",")</f>
+        <f t="shared" si="1"/>
         <v>foundation drift/.store in=\foundationdrift,</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\foundationdrift=\foundationdrift;</v>
       </c>
     </row>
@@ -1079,15 +1094,15 @@
         <v>36</v>
       </c>
       <c r="D11" t="str">
-        <f>CONCATENATE(A11,"=",C11,",")</f>
+        <f t="shared" si="0"/>
         <v>arrow tip length=3pt,</v>
       </c>
       <c r="E11" t="str">
-        <f>CONCATENATE(A11,"/.store in=", B11,",")</f>
+        <f t="shared" si="1"/>
         <v>arrow tip length/.store in=\arrlen,</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\arrlen=\arrlen;</v>
       </c>
     </row>
@@ -1102,15 +1117,15 @@
         <v>37</v>
       </c>
       <c r="D12" t="str">
-        <f>CONCATENATE(A12,"=",C12,",")</f>
+        <f t="shared" si="0"/>
         <v>arrow tip width=2pt,</v>
       </c>
       <c r="E12" t="str">
-        <f>CONCATENATE(A12,"/.store in=", B12,",")</f>
+        <f t="shared" si="1"/>
         <v>arrow tip width/.store in=\arrwid,</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\arrwid=\arrwid;</v>
       </c>
     </row>
@@ -1125,15 +1140,15 @@
         <v>42</v>
       </c>
       <c r="D13" t="str">
-        <f>CONCATENATE(A13,"=",C13,",")</f>
+        <f t="shared" si="0"/>
         <v>story to place superstructure dof=2,</v>
       </c>
       <c r="E13" t="str">
-        <f>CONCATENATE(A13,"/.store in=", B13,",")</f>
+        <f t="shared" si="1"/>
         <v>story to place superstructure dof/.store in=\doftextstory,</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\doftextstory=\doftextstory;</v>
       </c>
     </row>
@@ -1148,15 +1163,15 @@
         <v>38</v>
       </c>
       <c r="D14" t="str">
-        <f>CONCATENATE(A14,"=",C14,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the superstructure dof=$x_i(t)$,</v>
       </c>
       <c r="E14" t="str">
-        <f>CONCATENATE(A14,"/.store in=", B14,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the superstructure dof/.store in=\doftext,</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\doftext=\doftext;</v>
       </c>
     </row>
@@ -1171,15 +1186,15 @@
         <v>39</v>
       </c>
       <c r="D15" t="str">
-        <f>CONCATENATE(A15,"=",C15,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the isolation dof=$x_b(t)$,</v>
       </c>
       <c r="E15" t="str">
-        <f>CONCATENATE(A15,"/.store in=", B15,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the isolation dof/.store in=\isodoftext,</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\isodoftext=\isodoftext;</v>
       </c>
     </row>
@@ -1194,15 +1209,15 @@
         <v>40</v>
       </c>
       <c r="D16" t="str">
-        <f>CONCATENATE(A16,"=",C16,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the ground dof=$x_g(t)$,</v>
       </c>
       <c r="E16" t="str">
-        <f>CONCATENATE(A16,"/.store in=", B16,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the ground dof/.store in=\grounddoftext,</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\grounddoftext=\grounddoftext;</v>
       </c>
     </row>
@@ -1217,15 +1232,15 @@
         <v>45</v>
       </c>
       <c r="D17" t="str">
-        <f>CONCATENATE(A17,"=",C17,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the story mass=$m_i$,</v>
       </c>
       <c r="E17" t="str">
-        <f>CONCATENATE(A17,"/.store in=", B17,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the story mass/.store in=\storymasstext,</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\storymasstext=\storymasstext;</v>
       </c>
     </row>
@@ -1240,15 +1255,15 @@
         <v>46</v>
       </c>
       <c r="D18" t="str">
-        <f>CONCATENATE(A18,"=",C18,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the base slab mass=$m_b$,</v>
       </c>
       <c r="E18" t="str">
-        <f>CONCATENATE(A18,"/.store in=", B18,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the base slab mass/.store in=\basemasstext,</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\basemasstext=\basemasstext;</v>
       </c>
     </row>
@@ -1263,15 +1278,15 @@
         <v>52</v>
       </c>
       <c r="D19" t="str">
-        <f>CONCATENATE(A19,"=",C19,",")</f>
+        <f t="shared" si="0"/>
         <v>text for the story properties=$k_i,c_i$,</v>
       </c>
       <c r="E19" t="str">
-        <f>CONCATENATE(A19,"/.store in=", B19,",")</f>
+        <f t="shared" si="1"/>
         <v>text for the story properties/.store in=\storyproptext,</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>\storyproptext=\storyproptext;</v>
       </c>
     </row>
@@ -1285,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1334,11 +1349,11 @@
         <v>3</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D48" si="0">CONCATENATE(A2,"=",C2,",")</f>
+        <f t="shared" ref="D2:D42" si="0">CONCATENATE(A2,"=",C2,",")</f>
         <v>number of bays =3,</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E48" si="1">CONCATENATE(A2,"/.store in=", B2,",")</f>
+        <f t="shared" ref="E2:E42" si="1">CONCATENATE(A2,"/.store in=", B2,",")</f>
         <v>number of bays /.store in=\baynumber,</v>
       </c>
       <c r="F2" t="str">
@@ -2268,10 +2283,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" t="s">
         <v>147</v>
-      </c>
-      <c r="B43" t="s">
-        <v>153</v>
       </c>
       <c r="C43" s="2">
         <v>1</v>
@@ -2291,10 +2306,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
         <v>148</v>
-      </c>
-      <c r="B44" t="s">
-        <v>154</v>
       </c>
       <c r="C44" s="2">
         <v>5</v>
@@ -2314,10 +2329,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
         <v>149</v>
-      </c>
-      <c r="B45" t="s">
-        <v>155</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>58</v>
@@ -2337,10 +2352,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" t="s">
         <v>150</v>
-      </c>
-      <c r="B46" t="s">
-        <v>156</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>32</v>
@@ -2360,10 +2375,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
         <v>151</v>
-      </c>
-      <c r="B47" t="s">
-        <v>157</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>32</v>
@@ -2383,10 +2398,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" t="s">
         <v>152</v>
-      </c>
-      <c r="B48" t="s">
-        <v>158</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>54</v>
@@ -2412,66 +2427,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B1" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("  ",A1,"=",C1,",")</f>
+        <v xml:space="preserve">  x coordinate=0cm,</v>
+      </c>
+      <c r="E1" t="str">
+        <f>CONCATENATE("  ",A1,"/.store in=", B1,",")</f>
+        <v xml:space="preserve">  x coordinate/.store in=\coordinatex,</v>
+      </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE(B1,"=",B1,";")</f>
+        <v>\coordinatex=\coordinatex;</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D6" si="0">CONCATENATE("  ",A2,"=",C2,",")</f>
+        <v xml:space="preserve">  y coordinate=0cm,</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E6" si="1">CONCATENATE("  ",A2,"/.store in=", B2,",")</f>
+        <v xml:space="preserve">  y coordinate/.store in=\coordinatey,</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F6" si="2">CONCATENATE(B2,"=",B2,";")</f>
+        <v>\coordinatey=\coordinatey;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  pile depth=4cm,</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  pile depth/.store in=\pdepth,</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="2"/>
+        <v>\pdepth=\pdepth;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  pile diameter=0.5cm,</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  pile diameter/.store in=\pdiameter,</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>\pdiameter=\pdiameter;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  pile line thickness=1pt,</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  pile line thickness/.store in=\plinethick,</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>\plinethick=\plinethick;</v>
+      </c>
+      <c r="G5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>162</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">  fill color=gray,</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  fill color/.store in=\fillcolor,</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>\fillcolor=\fillcolor;</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>